<commit_message>
adicionando versão inicial do index
</commit_message>
<xml_diff>
--- a/documentacao/Backlog_LwC.xlsx
+++ b/documentacao/Backlog_LwC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Trabalho_PI_Semestral\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75651B05-BB75-4A31-ADDC-A53E28A31DC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A2347A-5AD2-4385-B535-4D0DDB115D8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -155,7 +155,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB2998C4-4D93-4C85-AAB7-E5F5E4E4B479}" name="Tabela1" displayName="Tabela1" ref="F2:I19" totalsRowShown="0">
   <autoFilter ref="F2:I19" xr:uid="{936C071F-F837-4822-A9B0-72944CE478BA}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F3:I19">
-    <sortCondition ref="I2:I19"/>
+    <sortCondition descending="1" ref="G2:G19"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{4C4173C9-8B04-4A70-A1AD-158E39210B9E}" name="Requisitos:"/>
@@ -433,7 +433,7 @@
   <dimension ref="F2:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,198 +460,198 @@
     </row>
     <row r="3" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4">
+        <v>13</v>
+      </c>
+      <c r="I4">
         <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
       </c>
     </row>
     <row r="5" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H5">
         <v>8</v>
       </c>
       <c r="I5">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
         <v>13</v>
       </c>
       <c r="H6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G7" t="s">
         <v>13</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G8" t="s">
         <v>13</v>
       </c>
       <c r="H8">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I8">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="G9" t="s">
         <v>13</v>
       </c>
       <c r="H9">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I9">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G10" t="s">
         <v>13</v>
       </c>
       <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
         <v>5</v>
-      </c>
-      <c r="I10">
-        <v>8</v>
       </c>
     </row>
     <row r="11" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
         <v>6</v>
-      </c>
-      <c r="G11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11">
-        <v>13</v>
-      </c>
-      <c r="I11">
-        <v>8</v>
       </c>
     </row>
     <row r="12" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12">
+        <v>8</v>
+      </c>
+      <c r="I12">
         <v>7</v>
-      </c>
-      <c r="G12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12">
-        <v>13</v>
-      </c>
-      <c r="I12">
-        <v>9</v>
       </c>
     </row>
     <row r="13" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="G13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H13">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="I13">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="G14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H14">
         <v>13</v>
       </c>
       <c r="I14">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G15" t="s">
         <v>13</v>
       </c>
       <c r="H15">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="I15">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G16" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H16">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="I16">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="6:9" x14ac:dyDescent="0.25">

</xml_diff>